<commit_message>
Services updated and new sql added
</commit_message>
<xml_diff>
--- a/FreeNForSaleServices/src/servlet/mvc/rest/database/Servces.xlsx
+++ b/FreeNForSaleServices/src/servlet/mvc/rest/database/Servces.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="109">
   <si>
     <t>Service</t>
   </si>
@@ -41,9 +42,6 @@
     <t>Op</t>
   </si>
   <si>
-    <t>FetchInventory</t>
-  </si>
-  <si>
     <t>Get</t>
   </si>
   <si>
@@ -68,9 +66,6 @@
     <t>itemID</t>
   </si>
   <si>
-    <t>ItemID,name,price,category,Primary Image(3  of each category)</t>
-  </si>
-  <si>
     <t>ItemId, name, Price, Description, All Images,category,category id</t>
   </si>
   <si>
@@ -137,9 +132,6 @@
     <t>GetCart</t>
   </si>
   <si>
-    <t>AddToCart</t>
-  </si>
-  <si>
     <t>cart Details</t>
   </si>
   <si>
@@ -210,6 +202,156 @@
   </si>
   <si>
     <t>{"1":[{"categoryId":1,"categoryName":"Furniture","inventoryName":"Table","itemId":1,"mainImage":null,"price":"8.75","remainingQuantity":1},{"categoryId":1,"categoryName":"Furniture","inventoryName":"Coupon","itemId":8,"mainImage":null,"price":"15.0","remainingQuantity":1}],"3":[{"categoryId":3,"categoryName":"Books","inventoryName":"Book - Statistics","itemId":4,"mainImage":null,"price":"27.0","remainingQuantity":1}],"5":[{"categoryId":5,"categoryName":"Electronics","inventoryName":"Laptop Screen","itemId":2,"mainImage":null,"price":"20.5","remainingQuantity":1},{"categoryId":5,"categoryName":"Electronics","inventoryName":"S5 cover","itemId":5,"mainImage":null,"price":"2.0","remainingQuantity":1}]}</t>
+  </si>
+  <si>
+    <t>{"inventoryId":"1","userId":"5","quantity":"1","amount":"8.75"}</t>
+  </si>
+  <si>
+    <t>https://localhost:8443/FreeNForSaleServices/rest/CartService/addToCart</t>
+  </si>
+  <si>
+    <t>/InventoryServices/InventoryForHomePage</t>
+  </si>
+  <si>
+    <t>This service fetches the list of different products.</t>
+  </si>
+  <si>
+    <t>No input</t>
+  </si>
+  <si>
+    <t>ProductID, Product Name, Cost, Image for all products</t>
+  </si>
+  <si>
+    <t>/InventoryServices/SearchInventory</t>
+  </si>
+  <si>
+    <t>The service returns the search results</t>
+  </si>
+  <si>
+    <t>/InventoryServices/FetchMoreDetails</t>
+  </si>
+  <si>
+    <t>The service returns details of individual product.</t>
+  </si>
+  <si>
+    <t>ProductID, Product Name,Price, Description, All Images</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>/loginservices/checkuservalidity</t>
+  </si>
+  <si>
+    <t>The service validates the user.</t>
+  </si>
+  <si>
+    <t>/registrationservices/newregistration</t>
+  </si>
+  <si>
+    <t>The service registers the user.</t>
+  </si>
+  <si>
+    <t>USerName, password, Name, Address</t>
+  </si>
+  <si>
+    <t>/profileservices/getprofile</t>
+  </si>
+  <si>
+    <t>The service gets Profile information</t>
+  </si>
+  <si>
+    <t>USerName, Name, Address</t>
+  </si>
+  <si>
+    <t>/profileservices/updateprofile</t>
+  </si>
+  <si>
+    <t>The service updates the profile information.</t>
+  </si>
+  <si>
+    <t>Success Message</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>/CartService/addToCart</t>
+  </si>
+  <si>
+    <t>The service adds the product to user cart.</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>/CartService/getCart</t>
+  </si>
+  <si>
+    <t>The service gets the cart details.</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Products in the cart</t>
+  </si>
+  <si>
+    <t>/CartService/saveUpdateCart</t>
+  </si>
+  <si>
+    <t>The service saves the carts.</t>
+  </si>
+  <si>
+    <t>/CartService/purchaseCart</t>
+  </si>
+  <si>
+    <t>The service purchase the products from the cart and sends the confirmation email</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>/TransactionService/getTransactionHistory</t>
+  </si>
+  <si>
+    <t>The service gets the transaction history of the user.</t>
+  </si>
+  <si>
+    <t>Past transaction data like items purchase, cost, date of purchase.</t>
+  </si>
+  <si>
+    <t>/ReviewServices/getReviews</t>
+  </si>
+  <si>
+    <t>The service gets the past review given by the user</t>
+  </si>
+  <si>
+    <t>/ReviewServices/saveReviews</t>
+  </si>
+  <si>
+    <t>ContactUS</t>
+  </si>
+  <si>
+    <t>/ContatcUsService/SendEmail</t>
+  </si>
+  <si>
+    <t>The service  saves the review.</t>
+  </si>
+  <si>
+    <t>The service sends the email for the message received confirmation.</t>
+  </si>
+  <si>
+    <t>emailId</t>
   </si>
 </sst>
 </file>
@@ -231,18 +373,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,14 +393,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,14 +690,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
@@ -563,14 +705,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -579,293 +721,685 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="A1:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="64.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>